<commit_message>
[ PUT ' / ' IF FIELD IS EMPTY ]
</commit_message>
<xml_diff>
--- a/dbc/EXPORT_CAN_EXTENDED/PowerTrain.xlsx
+++ b/dbc/EXPORT_CAN_EXTENDED/PowerTrain.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="93">
   <si>
     <t>Result</t>
   </si>
@@ -924,8 +924,12 @@
       <c r="AH2" s="2">
         <v>1</v>
       </c>
-      <c r="AI2" s="2"/>
-      <c r="AJ2" s="2"/>
+      <c r="AI2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="AK2" s="2" t="s">
         <v>42</v>
       </c>
@@ -935,7 +939,9 @@
       <c r="AM2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AN2" s="2"/>
+      <c r="AN2" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="AO2" s="2" t="s">
         <v>48</v>
       </c>
@@ -1046,8 +1052,12 @@
       <c r="AH3" s="2">
         <v>1</v>
       </c>
-      <c r="AI3" s="2"/>
-      <c r="AJ3" s="2"/>
+      <c r="AI3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AJ3" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="AK3" s="2" t="s">
         <v>42</v>
       </c>
@@ -1057,7 +1067,9 @@
       <c r="AM3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AN3" s="2"/>
+      <c r="AN3" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="AO3" s="2" t="s">
         <v>49</v>
       </c>
@@ -1168,8 +1180,12 @@
       <c r="AH4" s="2">
         <v>1</v>
       </c>
-      <c r="AI4" s="2"/>
-      <c r="AJ4" s="2"/>
+      <c r="AI4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AJ4" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="AK4" s="2" t="s">
         <v>42</v>
       </c>
@@ -1179,7 +1195,9 @@
       <c r="AM4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AN4" s="2"/>
+      <c r="AN4" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="AO4" s="2" t="s">
         <v>49</v>
       </c>
@@ -1290,8 +1308,12 @@
       <c r="AH5" s="2">
         <v>1</v>
       </c>
-      <c r="AI5" s="2"/>
-      <c r="AJ5" s="2"/>
+      <c r="AI5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AJ5" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="AK5" s="2" t="s">
         <v>42</v>
       </c>
@@ -1301,7 +1323,9 @@
       <c r="AM5" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AN5" s="2"/>
+      <c r="AN5" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="AO5" s="2" t="s">
         <v>49</v>
       </c>
@@ -1412,7 +1436,9 @@
       <c r="AH6" s="3">
         <v>0</v>
       </c>
-      <c r="AI6" s="3"/>
+      <c r="AI6" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="AJ6" s="3" t="s">
         <v>60</v>
       </c>
@@ -1425,7 +1451,9 @@
       <c r="AM6" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AN6" s="3"/>
+      <c r="AN6" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="AO6" s="3" t="s">
         <v>49</v>
       </c>
@@ -1536,7 +1564,9 @@
       <c r="AH7" s="3">
         <v>5</v>
       </c>
-      <c r="AI7" s="3"/>
+      <c r="AI7" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="AJ7" s="3" t="s">
         <v>62</v>
       </c>
@@ -1549,7 +1579,9 @@
       <c r="AM7" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AN7" s="3"/>
+      <c r="AN7" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="AO7" s="3" t="s">
         <v>49</v>
       </c>
@@ -1660,8 +1692,12 @@
       <c r="AH8" s="2">
         <v>0</v>
       </c>
-      <c r="AI8" s="2"/>
-      <c r="AJ8" s="2"/>
+      <c r="AI8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AJ8" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="AK8" s="2" t="s">
         <v>42</v>
       </c>
@@ -1671,7 +1707,9 @@
       <c r="AM8" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AN8" s="2"/>
+      <c r="AN8" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="AO8" s="2" t="s">
         <v>49</v>
       </c>
@@ -1782,7 +1820,9 @@
       <c r="AH9" s="3">
         <v>0</v>
       </c>
-      <c r="AI9" s="3"/>
+      <c r="AI9" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="AJ9" s="3" t="s">
         <v>67</v>
       </c>
@@ -1795,7 +1835,9 @@
       <c r="AM9" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AN9" s="3"/>
+      <c r="AN9" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="AO9" s="3" t="s">
         <v>49</v>
       </c>
@@ -1909,7 +1951,9 @@
       <c r="AI10" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="AJ10" s="2"/>
+      <c r="AJ10" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="AK10" s="2" t="s">
         <v>42</v>
       </c>
@@ -1919,7 +1963,9 @@
       <c r="AM10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AN10" s="2"/>
+      <c r="AN10" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="AO10" s="2" t="s">
         <v>49</v>
       </c>
@@ -2033,7 +2079,9 @@
       <c r="AI11" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AJ11" s="3"/>
+      <c r="AJ11" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="AK11" s="3" t="s">
         <v>42</v>
       </c>
@@ -2043,7 +2091,9 @@
       <c r="AM11" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AN11" s="3"/>
+      <c r="AN11" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="AO11" s="3" t="s">
         <v>49</v>
       </c>
@@ -2157,7 +2207,9 @@
       <c r="AI12" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AJ12" s="2"/>
+      <c r="AJ12" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="AK12" s="2" t="s">
         <v>42</v>
       </c>
@@ -2167,7 +2219,9 @@
       <c r="AM12" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AN12" s="2"/>
+      <c r="AN12" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="AO12" s="2" t="s">
         <v>49</v>
       </c>
@@ -2281,7 +2335,9 @@
       <c r="AI13" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="AJ13" s="3"/>
+      <c r="AJ13" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="AK13" s="3" t="s">
         <v>42</v>
       </c>
@@ -2291,7 +2347,9 @@
       <c r="AM13" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AN13" s="3"/>
+      <c r="AN13" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="AO13" s="3" t="s">
         <v>49</v>
       </c>
@@ -2405,7 +2463,9 @@
       <c r="AI14" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AJ14" s="3"/>
+      <c r="AJ14" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="AK14" s="3" t="s">
         <v>42</v>
       </c>
@@ -2415,7 +2475,9 @@
       <c r="AM14" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AN14" s="3"/>
+      <c r="AN14" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="AO14" s="3" t="s">
         <v>49</v>
       </c>
@@ -2526,7 +2588,9 @@
       <c r="AH15" s="3">
         <v>0</v>
       </c>
-      <c r="AI15" s="3"/>
+      <c r="AI15" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="AJ15" s="3" t="s">
         <v>82</v>
       </c>
@@ -2539,7 +2603,9 @@
       <c r="AM15" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AN15" s="3"/>
+      <c r="AN15" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="AO15" s="3" t="s">
         <v>49</v>
       </c>
@@ -2653,7 +2719,9 @@
       <c r="AI16" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="AJ16" s="3"/>
+      <c r="AJ16" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="AK16" s="3" t="s">
         <v>42</v>
       </c>
@@ -2663,7 +2731,9 @@
       <c r="AM16" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AN16" s="3"/>
+      <c r="AN16" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="AO16" s="3" t="s">
         <v>49</v>
       </c>
@@ -2777,7 +2847,9 @@
       <c r="AI17" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="AJ17" s="3"/>
+      <c r="AJ17" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="AK17" s="3" t="s">
         <v>42</v>
       </c>
@@ -2787,7 +2859,9 @@
       <c r="AM17" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AN17" s="3"/>
+      <c r="AN17" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="AO17" s="3" t="s">
         <v>49</v>
       </c>
@@ -2901,7 +2975,9 @@
       <c r="AI18" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="AJ18" s="2"/>
+      <c r="AJ18" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="AK18" s="2" t="s">
         <v>42</v>
       </c>
@@ -2911,7 +2987,9 @@
       <c r="AM18" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AN18" s="2"/>
+      <c r="AN18" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="AO18" s="2" t="s">
         <v>49</v>
       </c>
@@ -3022,8 +3100,12 @@
       <c r="AH19" s="3">
         <v>0</v>
       </c>
-      <c r="AI19" s="3"/>
-      <c r="AJ19" s="3"/>
+      <c r="AI19" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AJ19" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="AK19" s="3" t="s">
         <v>42</v>
       </c>
@@ -3033,7 +3115,9 @@
       <c r="AM19" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AN19" s="3"/>
+      <c r="AN19" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="AO19" s="3" t="s">
         <v>49</v>
       </c>
@@ -3144,7 +3228,9 @@
       <c r="AH20" s="3">
         <v>0</v>
       </c>
-      <c r="AI20" s="3"/>
+      <c r="AI20" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="AJ20" s="3" t="s">
         <v>90</v>
       </c>
@@ -3157,7 +3243,9 @@
       <c r="AM20" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AN20" s="3"/>
+      <c r="AN20" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="AO20" s="3" t="s">
         <v>49</v>
       </c>
@@ -3271,7 +3359,9 @@
       <c r="AI21" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="AJ21" s="3"/>
+      <c r="AJ21" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="AK21" s="3" t="s">
         <v>42</v>
       </c>
@@ -3281,7 +3371,9 @@
       <c r="AM21" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AN21" s="3"/>
+      <c r="AN21" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="AO21" s="3" t="s">
         <v>49</v>
       </c>

</xml_diff>